<commit_message>
finished missing acceptors and donors
</commit_message>
<xml_diff>
--- a/ml_for_opvs/data/preprocess/OPV_Min/clean_min_acceptors.xlsx
+++ b/ml_for_opvs/data/preprocess/OPV_Min/clean_min_acceptors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanley Lo\Documents\Summer 2021 NSERC\opv_ml\opv_ml\data\preprocess\OPV_Min\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanley Lo\Documents\Summer 2021 NSERC\ml_for_opvs\ml_for_opvs\data\preprocess\OPV_Min\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7A8808D-2229-44C3-8F6E-BD1D7C3442FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEBC038-B6ED-4B2B-98F0-258B9AAC973B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896"/>
+    <workbookView xWindow="276" yWindow="1092" windowWidth="28800" windowHeight="15072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clean_min_acceptors" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1659" uniqueCount="1297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="1292">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -1373,21 +1373,6 @@
   </si>
   <si>
     <t>[C][C][C][C][C][C][C][=C][C][=C][Branch2_1][N][Branch1_2][C][Branch1_1][P][C][=C][C][=C][Branch1_1][Branch1_3][C][C][C][C][C][C][C][=C][Ring1][N][C][=C][Branch2_1][Ring2][O][S][C][C][=C][Branch2_1][Ring1][N][C][=C][C][Branch1_2][C][=O][C][=C][C][Branch1_1][C][F][=C][C][=C][Ring1][Branch1_3][C][Ring1][O][=C][Branch1_1][Ring1][C][#N][C][#N][S][C][Ring2][Ring1][Branch2_2][Expl=Ring2][Ring1][Branch1_2][C][S][C][C][=C][Branch1_1][O][S][C][Expl=Ring1][Branch1_1][C][Expl=Ring1][Branch2_1][Ring2][Ring2][=C][C][S][C][C][=C][Branch2_1][Ring1][N][C][=C][C][Branch1_2][C][=O][C][=C][C][Branch1_1][C][F][=C][C][=C][Ring1][Branch1_3][C][Ring1][O][=C][Branch1_1][Ring1][C][#N][C][#N][S][C][Expl=Ring2][Ring1][Branch1_2][C][Expl=Ring2][Ring1][Branch2_2][C][Ring2][Ring1][#C][Branch1_1][P][C][=C][C][=C][Branch1_1][Branch1_3][C][C][C][C][C][C][C][=C][Ring1][N][C][=C][C][=C][Branch1_1][Branch1_3][C][C][C][C][C][C][C][=C][Ring1][N][C][=C][Ring2][Branch2_1][Branch1_2]</t>
-  </si>
-  <si>
-    <t>N5</t>
-  </si>
-  <si>
-    <t>CCCCCCCC[Si]1(CCCCCCCC)c2cc(-c3ccc(/C=C4\C(=O)c5ccccc5C4=C(C#N)C#N)s3)ccc2-c2ccc(-c3ccc(/C=C4\C(=O)c5ccccc5C4=C(C#N)C#N)s3)cc21</t>
-  </si>
-  <si>
-    <t>O=C1c2c(C(/C1=C/c1ccc(c3cc([Si]4([R2])[R2])c(c5c4cc(c4sc(/C=C6C(c7ccccc7C\6=C(C#N)\C#N)=O)cc4)cc5)cc3)s1)=C(C#N)\C#N)cccc2</t>
-  </si>
-  <si>
-    <t>{([$])CCCCCCC[Si]1(CCCCCCCC)c2cc(-c3ccc(/C=C4\C(=O)c5ccccc5C4=C(C#N)C#N)s3)ccc2-c2ccc(-c3ccc(/C=C4\C(=O)c5ccccc5C4=C(C#N)C#N)s3)cc21}</t>
-  </si>
-  <si>
-    <t>[C][C][C][C][C][C][C][C][Siexpl][Branch1_1][Branch2_2][C][C][C][C][C][C][C][C][C][=C][C][Branch2_1][Ring2][Ring2][C][=C][C][=C][Branch2_1][Ring1][Branch2_2][/C][=C][\C][Branch1_2][C][=O][C][=C][C][=C][C][=C][Ring1][Branch1_2][C][Ring1][Branch2_3][=C][Branch1_1][Ring1][C][#N][C][#N][S][Ring2][Ring1][Branch1_1][=C][C][=C][Ring2][Ring1][O][C][=C][C][=C][Branch2_1][Ring2][Ring2][C][=C][C][=C][Branch2_1][Ring1][Branch2_2][/C][=C][\C][Branch1_2][C][=O][C][=C][C][=C][C][=C][Ring1][Branch1_2][C][Ring1][Branch2_3][=C][Branch1_1][Ring1][C][#N][C][#N][S][Ring2][Ring1][Branch1_1][C][=C][Ring2][Ring1][O][Ring2][Branch1_1][#C]</t>
   </si>
   <si>
     <t>IT-O1</t>
@@ -3916,7 +3901,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4761,11 +4746,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G277"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G276"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="C176" sqref="C176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6905,7 +6890,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B94" t="s">
         <v>451</v>
@@ -6928,7 +6913,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B95" t="s">
         <v>456</v>
@@ -6951,7 +6936,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B96" t="s">
         <v>461</v>
@@ -6974,7 +6959,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B97" t="s">
         <v>466</v>
@@ -6997,7 +6982,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B98" t="s">
         <v>471</v>
@@ -7020,7 +7005,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B99" t="s">
         <v>476</v>
@@ -7043,7 +7028,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B100" t="s">
         <v>481</v>
@@ -7066,7 +7051,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B101" t="s">
         <v>486</v>
@@ -7089,7 +7074,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B102" t="s">
         <v>491</v>
@@ -7112,7 +7097,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B103" t="s">
         <v>496</v>
@@ -7135,7 +7120,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B104" t="s">
         <v>501</v>
@@ -7158,73 +7143,73 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B105" t="s">
         <v>506</v>
       </c>
       <c r="C105" t="s">
+        <v>179</v>
+      </c>
+      <c r="D105" t="s">
         <v>507</v>
       </c>
-      <c r="D105" t="s">
-        <v>508</v>
-      </c>
       <c r="E105" t="s">
         <v>10</v>
       </c>
       <c r="F105" t="s">
-        <v>509</v>
+        <v>181</v>
       </c>
       <c r="G105" t="s">
-        <v>510</v>
+        <v>182</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>104</v>
-      </c>
-      <c r="B106" t="s">
-        <v>511</v>
+        <v>105</v>
       </c>
       <c r="C106" t="s">
-        <v>179</v>
+        <v>239</v>
       </c>
       <c r="D106" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="E106" t="s">
         <v>10</v>
       </c>
       <c r="F106" t="s">
-        <v>181</v>
+        <v>241</v>
       </c>
       <c r="G106" t="s">
-        <v>182</v>
+        <v>242</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>105</v>
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>509</v>
       </c>
       <c r="C107" t="s">
-        <v>239</v>
+        <v>510</v>
       </c>
       <c r="D107" t="s">
+        <v>511</v>
+      </c>
+      <c r="E107" t="s">
+        <v>10</v>
+      </c>
+      <c r="F107" t="s">
+        <v>512</v>
+      </c>
+      <c r="G107" t="s">
         <v>513</v>
-      </c>
-      <c r="E107" t="s">
-        <v>10</v>
-      </c>
-      <c r="F107" t="s">
-        <v>241</v>
-      </c>
-      <c r="G107" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B108" t="s">
         <v>514</v>
@@ -7247,7 +7232,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B109" t="s">
         <v>519</v>
@@ -7270,7 +7255,7 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B110" t="s">
         <v>524</v>
@@ -7293,7 +7278,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B111" t="s">
         <v>529</v>
@@ -7316,53 +7301,53 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B112" t="s">
         <v>534</v>
       </c>
       <c r="C112" t="s">
+        <v>422</v>
+      </c>
+      <c r="D112" t="s">
         <v>535</v>
       </c>
-      <c r="D112" t="s">
-        <v>536</v>
-      </c>
       <c r="E112" t="s">
         <v>10</v>
       </c>
       <c r="F112" t="s">
-        <v>537</v>
+        <v>424</v>
       </c>
       <c r="G112" t="s">
-        <v>538</v>
+        <v>425</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B113" t="s">
+        <v>536</v>
+      </c>
+      <c r="C113" t="s">
+        <v>537</v>
+      </c>
+      <c r="D113" t="s">
+        <v>538</v>
+      </c>
+      <c r="E113" t="s">
+        <v>10</v>
+      </c>
+      <c r="F113" t="s">
         <v>539</v>
       </c>
-      <c r="C113" t="s">
-        <v>422</v>
-      </c>
-      <c r="D113" t="s">
+      <c r="G113" t="s">
         <v>540</v>
-      </c>
-      <c r="E113" t="s">
-        <v>10</v>
-      </c>
-      <c r="F113" t="s">
-        <v>424</v>
-      </c>
-      <c r="G113" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B114" t="s">
         <v>541</v>
@@ -7385,7 +7370,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B115" t="s">
         <v>546</v>
@@ -7408,7 +7393,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B116" t="s">
         <v>551</v>
@@ -7431,7 +7416,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B117" t="s">
         <v>556</v>
@@ -7454,7 +7439,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B118" t="s">
         <v>561</v>
@@ -7477,53 +7462,53 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B119" t="s">
         <v>566</v>
       </c>
       <c r="C119" t="s">
+        <v>300</v>
+      </c>
+      <c r="D119" t="s">
         <v>567</v>
       </c>
-      <c r="D119" t="s">
-        <v>568</v>
-      </c>
       <c r="E119" t="s">
         <v>10</v>
       </c>
       <c r="F119" t="s">
-        <v>569</v>
+        <v>302</v>
       </c>
       <c r="G119" t="s">
-        <v>570</v>
+        <v>303</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B120" t="s">
+        <v>568</v>
+      </c>
+      <c r="C120" t="s">
+        <v>569</v>
+      </c>
+      <c r="D120" t="s">
+        <v>570</v>
+      </c>
+      <c r="E120" t="s">
+        <v>10</v>
+      </c>
+      <c r="F120" t="s">
         <v>571</v>
       </c>
-      <c r="C120" t="s">
-        <v>300</v>
-      </c>
-      <c r="D120" t="s">
+      <c r="G120" t="s">
         <v>572</v>
-      </c>
-      <c r="E120" t="s">
-        <v>10</v>
-      </c>
-      <c r="F120" t="s">
-        <v>302</v>
-      </c>
-      <c r="G120" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B121" t="s">
         <v>573</v>
@@ -7546,7 +7531,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B122" t="s">
         <v>578</v>
@@ -7569,7 +7554,7 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B123" t="s">
         <v>583</v>
@@ -7592,7 +7577,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B124" t="s">
         <v>588</v>
@@ -7615,7 +7600,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B125" t="s">
         <v>593</v>
@@ -7638,53 +7623,53 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B126" t="s">
         <v>598</v>
       </c>
       <c r="C126" t="s">
+        <v>234</v>
+      </c>
+      <c r="D126" t="s">
         <v>599</v>
       </c>
-      <c r="D126" t="s">
-        <v>600</v>
-      </c>
       <c r="E126" t="s">
         <v>10</v>
       </c>
       <c r="F126" t="s">
-        <v>601</v>
+        <v>236</v>
       </c>
       <c r="G126" t="s">
-        <v>602</v>
+        <v>237</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B127" t="s">
+        <v>600</v>
+      </c>
+      <c r="C127" t="s">
+        <v>601</v>
+      </c>
+      <c r="D127" t="s">
+        <v>602</v>
+      </c>
+      <c r="E127" t="s">
+        <v>10</v>
+      </c>
+      <c r="F127" t="s">
         <v>603</v>
       </c>
-      <c r="C127" t="s">
-        <v>234</v>
-      </c>
-      <c r="D127" t="s">
+      <c r="G127" t="s">
         <v>604</v>
-      </c>
-      <c r="E127" t="s">
-        <v>10</v>
-      </c>
-      <c r="F127" t="s">
-        <v>236</v>
-      </c>
-      <c r="G127" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B128" t="s">
         <v>605</v>
@@ -7707,7 +7692,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B129" t="s">
         <v>610</v>
@@ -7730,7 +7715,7 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B130" t="s">
         <v>615</v>
@@ -7753,7 +7738,7 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B131" t="s">
         <v>620</v>
@@ -7776,7 +7761,7 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B132" t="s">
         <v>625</v>
@@ -7799,7 +7784,7 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B133" t="s">
         <v>630</v>
@@ -7822,7 +7807,7 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B134" t="s">
         <v>635</v>
@@ -7845,7 +7830,7 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B135" t="s">
         <v>640</v>
@@ -7868,53 +7853,53 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B136" t="s">
         <v>645</v>
       </c>
       <c r="C136" t="s">
+        <v>194</v>
+      </c>
+      <c r="D136" t="s">
         <v>646</v>
       </c>
-      <c r="D136" t="s">
-        <v>647</v>
-      </c>
       <c r="E136" t="s">
         <v>10</v>
       </c>
       <c r="F136" t="s">
-        <v>648</v>
+        <v>196</v>
       </c>
       <c r="G136" t="s">
-        <v>649</v>
+        <v>197</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B137" t="s">
+        <v>647</v>
+      </c>
+      <c r="C137" t="s">
+        <v>648</v>
+      </c>
+      <c r="D137" t="s">
+        <v>649</v>
+      </c>
+      <c r="E137" t="s">
+        <v>10</v>
+      </c>
+      <c r="F137" t="s">
         <v>650</v>
       </c>
-      <c r="C137" t="s">
-        <v>194</v>
-      </c>
-      <c r="D137" t="s">
+      <c r="G137" t="s">
         <v>651</v>
-      </c>
-      <c r="E137" t="s">
-        <v>10</v>
-      </c>
-      <c r="F137" t="s">
-        <v>196</v>
-      </c>
-      <c r="G137" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B138" t="s">
         <v>652</v>
@@ -7937,53 +7922,53 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B139" t="s">
         <v>657</v>
       </c>
       <c r="C139" t="s">
+        <v>584</v>
+      </c>
+      <c r="D139" t="s">
         <v>658</v>
       </c>
-      <c r="D139" t="s">
-        <v>659</v>
-      </c>
       <c r="E139" t="s">
         <v>10</v>
       </c>
       <c r="F139" t="s">
-        <v>660</v>
+        <v>586</v>
       </c>
       <c r="G139" t="s">
-        <v>661</v>
+        <v>587</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B140" t="s">
+        <v>659</v>
+      </c>
+      <c r="C140" t="s">
+        <v>660</v>
+      </c>
+      <c r="D140" t="s">
+        <v>661</v>
+      </c>
+      <c r="E140" t="s">
+        <v>10</v>
+      </c>
+      <c r="F140" t="s">
         <v>662</v>
       </c>
-      <c r="C140" t="s">
-        <v>589</v>
-      </c>
-      <c r="D140" t="s">
+      <c r="G140" t="s">
         <v>663</v>
-      </c>
-      <c r="E140" t="s">
-        <v>10</v>
-      </c>
-      <c r="F140" t="s">
-        <v>591</v>
-      </c>
-      <c r="G140" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B141" t="s">
         <v>664</v>
@@ -8006,7 +7991,7 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B142" t="s">
         <v>669</v>
@@ -8029,7 +8014,7 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B143" t="s">
         <v>674</v>
@@ -8052,7 +8037,7 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B144" t="s">
         <v>679</v>
@@ -8075,7 +8060,7 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B145" t="s">
         <v>684</v>
@@ -8098,99 +8083,99 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B146" t="s">
         <v>689</v>
       </c>
       <c r="C146" t="s">
+        <v>119</v>
+      </c>
+      <c r="D146" t="s">
         <v>690</v>
       </c>
-      <c r="D146" t="s">
-        <v>691</v>
-      </c>
       <c r="E146" t="s">
         <v>10</v>
       </c>
       <c r="F146" t="s">
-        <v>692</v>
+        <v>121</v>
       </c>
       <c r="G146" t="s">
-        <v>693</v>
+        <v>122</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B147" t="s">
+        <v>691</v>
+      </c>
+      <c r="C147" t="s">
+        <v>692</v>
+      </c>
+      <c r="D147" t="s">
+        <v>693</v>
+      </c>
+      <c r="E147" t="s">
+        <v>10</v>
+      </c>
+      <c r="F147" t="s">
         <v>694</v>
       </c>
-      <c r="C147" t="s">
-        <v>119</v>
-      </c>
-      <c r="D147" t="s">
+      <c r="G147" t="s">
         <v>695</v>
-      </c>
-      <c r="E147" t="s">
-        <v>10</v>
-      </c>
-      <c r="F147" t="s">
-        <v>121</v>
-      </c>
-      <c r="G147" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B148" t="s">
         <v>696</v>
       </c>
       <c r="C148" t="s">
+        <v>234</v>
+      </c>
+      <c r="D148" t="s">
         <v>697</v>
       </c>
-      <c r="D148" t="s">
-        <v>698</v>
-      </c>
       <c r="E148" t="s">
         <v>10</v>
       </c>
       <c r="F148" t="s">
-        <v>699</v>
+        <v>236</v>
       </c>
       <c r="G148" t="s">
-        <v>700</v>
+        <v>237</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B149" t="s">
+        <v>698</v>
+      </c>
+      <c r="C149" t="s">
+        <v>699</v>
+      </c>
+      <c r="D149" t="s">
+        <v>700</v>
+      </c>
+      <c r="E149" t="s">
+        <v>10</v>
+      </c>
+      <c r="F149" t="s">
         <v>701</v>
       </c>
-      <c r="C149" t="s">
-        <v>234</v>
-      </c>
-      <c r="D149" t="s">
+      <c r="G149" t="s">
         <v>702</v>
-      </c>
-      <c r="E149" t="s">
-        <v>10</v>
-      </c>
-      <c r="F149" t="s">
-        <v>236</v>
-      </c>
-      <c r="G149" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B150" t="s">
         <v>703</v>
@@ -8213,53 +8198,53 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B151" t="s">
         <v>708</v>
       </c>
       <c r="C151" t="s">
-        <v>709</v>
+        <v>452</v>
       </c>
       <c r="D151" t="s">
-        <v>710</v>
+        <v>453</v>
       </c>
       <c r="E151" t="s">
         <v>10</v>
       </c>
       <c r="F151" t="s">
-        <v>711</v>
+        <v>454</v>
       </c>
       <c r="G151" t="s">
-        <v>712</v>
+        <v>455</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B152" t="s">
+        <v>709</v>
+      </c>
+      <c r="C152" t="s">
+        <v>710</v>
+      </c>
+      <c r="D152" t="s">
+        <v>711</v>
+      </c>
+      <c r="E152" t="s">
+        <v>10</v>
+      </c>
+      <c r="F152" t="s">
+        <v>712</v>
+      </c>
+      <c r="G152" t="s">
         <v>713</v>
-      </c>
-      <c r="C152" t="s">
-        <v>457</v>
-      </c>
-      <c r="D152" t="s">
-        <v>458</v>
-      </c>
-      <c r="E152" t="s">
-        <v>10</v>
-      </c>
-      <c r="F152" t="s">
-        <v>459</v>
-      </c>
-      <c r="G152" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B153" t="s">
         <v>714</v>
@@ -8282,7 +8267,7 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B154" t="s">
         <v>719</v>
@@ -8305,7 +8290,7 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B155" t="s">
         <v>724</v>
@@ -8328,7 +8313,7 @@
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B156" t="s">
         <v>729</v>
@@ -8351,7 +8336,7 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B157" t="s">
         <v>734</v>
@@ -8374,7 +8359,7 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B158" t="s">
         <v>739</v>
@@ -8397,7 +8382,7 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B159" t="s">
         <v>744</v>
@@ -8420,53 +8405,53 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B160" t="s">
         <v>749</v>
       </c>
       <c r="C160" t="s">
+        <v>164</v>
+      </c>
+      <c r="D160" t="s">
         <v>750</v>
       </c>
-      <c r="D160" t="s">
-        <v>751</v>
-      </c>
       <c r="E160" t="s">
         <v>10</v>
       </c>
       <c r="F160" t="s">
-        <v>752</v>
+        <v>166</v>
       </c>
       <c r="G160" t="s">
-        <v>753</v>
+        <v>167</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B161" t="s">
+        <v>751</v>
+      </c>
+      <c r="C161" t="s">
+        <v>752</v>
+      </c>
+      <c r="D161" t="s">
+        <v>753</v>
+      </c>
+      <c r="E161" t="s">
+        <v>10</v>
+      </c>
+      <c r="F161" t="s">
         <v>754</v>
       </c>
-      <c r="C161" t="s">
-        <v>164</v>
-      </c>
-      <c r="D161" t="s">
+      <c r="G161" t="s">
         <v>755</v>
-      </c>
-      <c r="E161" t="s">
-        <v>10</v>
-      </c>
-      <c r="F161" t="s">
-        <v>166</v>
-      </c>
-      <c r="G161" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B162" t="s">
         <v>756</v>
@@ -8489,7 +8474,7 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B163" t="s">
         <v>761</v>
@@ -8512,7 +8497,7 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B164" t="s">
         <v>766</v>
@@ -8535,7 +8520,7 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B165" t="s">
         <v>771</v>
@@ -8558,7 +8543,7 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B166" t="s">
         <v>776</v>
@@ -8581,7 +8566,7 @@
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B167" t="s">
         <v>781</v>
@@ -8604,7 +8589,7 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B168" t="s">
         <v>786</v>
@@ -8627,7 +8612,7 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B169" t="s">
         <v>791</v>
@@ -8650,7 +8635,7 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B170" t="s">
         <v>796</v>
@@ -8673,7 +8658,7 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B171" t="s">
         <v>801</v>
@@ -8696,7 +8681,7 @@
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B172" t="s">
         <v>806</v>
@@ -8719,7 +8704,7 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A173">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B173" t="s">
         <v>811</v>
@@ -8742,7 +8727,7 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A174">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B174" t="s">
         <v>816</v>
@@ -8765,7 +8750,7 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B175" t="s">
         <v>821</v>
@@ -8788,7 +8773,7 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A176">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B176" t="s">
         <v>826</v>
@@ -8811,7 +8796,7 @@
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A177">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B177" t="s">
         <v>831</v>
@@ -8834,7 +8819,7 @@
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A178">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B178" t="s">
         <v>836</v>
@@ -8857,7 +8842,7 @@
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A179">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B179" t="s">
         <v>841</v>
@@ -8880,7 +8865,7 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A180">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B180" t="s">
         <v>846</v>
@@ -8903,7 +8888,7 @@
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A181">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B181" t="s">
         <v>851</v>
@@ -8926,7 +8911,7 @@
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A182">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B182" t="s">
         <v>856</v>
@@ -8949,73 +8934,73 @@
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A183">
-        <v>181</v>
-      </c>
-      <c r="B183" t="s">
+        <v>182</v>
+      </c>
+      <c r="C183" t="s">
+        <v>79</v>
+      </c>
+      <c r="D183" t="s">
         <v>861</v>
       </c>
-      <c r="C183" t="s">
-        <v>862</v>
-      </c>
-      <c r="D183" t="s">
-        <v>863</v>
-      </c>
       <c r="E183" t="s">
         <v>10</v>
       </c>
       <c r="F183" t="s">
-        <v>864</v>
+        <v>81</v>
       </c>
       <c r="G183" t="s">
-        <v>865</v>
+        <v>82</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A184">
-        <v>182</v>
+        <v>183</v>
+      </c>
+      <c r="B184" t="s">
+        <v>862</v>
       </c>
       <c r="C184" t="s">
-        <v>79</v>
+        <v>355</v>
       </c>
       <c r="D184" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="E184" t="s">
         <v>10</v>
       </c>
       <c r="F184" t="s">
-        <v>81</v>
+        <v>357</v>
       </c>
       <c r="G184" t="s">
-        <v>82</v>
+        <v>358</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A185">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B185" t="s">
+        <v>864</v>
+      </c>
+      <c r="C185" t="s">
+        <v>865</v>
+      </c>
+      <c r="D185" t="s">
+        <v>866</v>
+      </c>
+      <c r="E185" t="s">
+        <v>10</v>
+      </c>
+      <c r="F185" t="s">
         <v>867</v>
       </c>
-      <c r="C185" t="s">
-        <v>355</v>
-      </c>
-      <c r="D185" t="s">
+      <c r="G185" t="s">
         <v>868</v>
-      </c>
-      <c r="E185" t="s">
-        <v>10</v>
-      </c>
-      <c r="F185" t="s">
-        <v>357</v>
-      </c>
-      <c r="G185" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A186">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B186" t="s">
         <v>869</v>
@@ -9038,7 +9023,7 @@
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A187">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B187" t="s">
         <v>874</v>
@@ -9061,7 +9046,7 @@
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A188">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B188" t="s">
         <v>879</v>
@@ -9084,53 +9069,53 @@
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A189">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B189" t="s">
         <v>884</v>
       </c>
       <c r="C189" t="s">
-        <v>885</v>
+        <v>300</v>
       </c>
       <c r="D189" t="s">
-        <v>886</v>
+        <v>301</v>
       </c>
       <c r="E189" t="s">
         <v>10</v>
       </c>
       <c r="F189" t="s">
-        <v>887</v>
+        <v>302</v>
       </c>
       <c r="G189" t="s">
-        <v>888</v>
+        <v>303</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A190">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B190" t="s">
+        <v>885</v>
+      </c>
+      <c r="C190" t="s">
+        <v>886</v>
+      </c>
+      <c r="D190" t="s">
+        <v>887</v>
+      </c>
+      <c r="E190" t="s">
+        <v>10</v>
+      </c>
+      <c r="F190" t="s">
+        <v>888</v>
+      </c>
+      <c r="G190" t="s">
         <v>889</v>
-      </c>
-      <c r="C190" t="s">
-        <v>300</v>
-      </c>
-      <c r="D190" t="s">
-        <v>301</v>
-      </c>
-      <c r="E190" t="s">
-        <v>10</v>
-      </c>
-      <c r="F190" t="s">
-        <v>302</v>
-      </c>
-      <c r="G190" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A191">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B191" t="s">
         <v>890</v>
@@ -9153,7 +9138,7 @@
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A192">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B192" t="s">
         <v>895</v>
@@ -9176,7 +9161,7 @@
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A193">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B193" t="s">
         <v>900</v>
@@ -9199,7 +9184,7 @@
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A194">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B194" t="s">
         <v>905</v>
@@ -9222,7 +9207,7 @@
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A195">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B195" t="s">
         <v>910</v>
@@ -9245,7 +9230,7 @@
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A196">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B196" t="s">
         <v>915</v>
@@ -9268,7 +9253,7 @@
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A197">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B197" t="s">
         <v>920</v>
@@ -9291,7 +9276,7 @@
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A198">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B198" t="s">
         <v>925</v>
@@ -9314,7 +9299,7 @@
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A199">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B199" t="s">
         <v>930</v>
@@ -9337,7 +9322,7 @@
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A200">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B200" t="s">
         <v>935</v>
@@ -9360,7 +9345,7 @@
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A201">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B201" t="s">
         <v>940</v>
@@ -9383,7 +9368,7 @@
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A202">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B202" t="s">
         <v>945</v>
@@ -9406,7 +9391,7 @@
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A203">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B203" t="s">
         <v>950</v>
@@ -9429,7 +9414,7 @@
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A204">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B204" t="s">
         <v>955</v>
@@ -9452,53 +9437,53 @@
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A205">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B205" t="s">
         <v>960</v>
       </c>
       <c r="C205" t="s">
+        <v>214</v>
+      </c>
+      <c r="D205" t="s">
         <v>961</v>
       </c>
-      <c r="D205" t="s">
-        <v>962</v>
-      </c>
       <c r="E205" t="s">
         <v>10</v>
       </c>
       <c r="F205" t="s">
-        <v>963</v>
+        <v>216</v>
       </c>
       <c r="G205" t="s">
-        <v>964</v>
+        <v>217</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A206">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B206" t="s">
+        <v>962</v>
+      </c>
+      <c r="C206" t="s">
+        <v>963</v>
+      </c>
+      <c r="D206" t="s">
+        <v>964</v>
+      </c>
+      <c r="E206" t="s">
+        <v>10</v>
+      </c>
+      <c r="F206" t="s">
         <v>965</v>
       </c>
-      <c r="C206" t="s">
-        <v>214</v>
-      </c>
-      <c r="D206" t="s">
+      <c r="G206" t="s">
         <v>966</v>
-      </c>
-      <c r="E206" t="s">
-        <v>10</v>
-      </c>
-      <c r="F206" t="s">
-        <v>216</v>
-      </c>
-      <c r="G206" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A207">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B207" t="s">
         <v>967</v>
@@ -9521,7 +9506,7 @@
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A208">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B208" t="s">
         <v>972</v>
@@ -9544,7 +9529,7 @@
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A209">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B209" t="s">
         <v>977</v>
@@ -9567,7 +9552,7 @@
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A210">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B210" t="s">
         <v>982</v>
@@ -9590,7 +9575,7 @@
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A211">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B211" t="s">
         <v>987</v>
@@ -9613,7 +9598,7 @@
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A212">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B212" t="s">
         <v>992</v>
@@ -9636,7 +9621,7 @@
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A213">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B213" t="s">
         <v>997</v>
@@ -9659,76 +9644,76 @@
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A214">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B214" t="s">
         <v>1002</v>
       </c>
       <c r="C214" t="s">
+        <v>89</v>
+      </c>
+      <c r="D214" t="s">
         <v>1003</v>
       </c>
-      <c r="D214" t="s">
-        <v>1004</v>
-      </c>
       <c r="E214" t="s">
         <v>10</v>
       </c>
       <c r="F214" t="s">
-        <v>1005</v>
+        <v>91</v>
       </c>
       <c r="G214" t="s">
-        <v>1006</v>
+        <v>92</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A215">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="C215" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="D215" t="s">
-        <v>1008</v>
+        <v>130</v>
       </c>
       <c r="E215" t="s">
         <v>10</v>
       </c>
       <c r="F215" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="G215" t="s">
-        <v>92</v>
+        <v>132</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A216">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B216" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C216" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D216" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E216" t="s">
+        <v>10</v>
+      </c>
+      <c r="F216" t="s">
+        <v>1008</v>
+      </c>
+      <c r="G216" t="s">
         <v>1009</v>
-      </c>
-      <c r="C216" t="s">
-        <v>129</v>
-      </c>
-      <c r="D216" t="s">
-        <v>130</v>
-      </c>
-      <c r="E216" t="s">
-        <v>10</v>
-      </c>
-      <c r="F216" t="s">
-        <v>131</v>
-      </c>
-      <c r="G216" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A217">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B217" t="s">
         <v>1010</v>
@@ -9751,7 +9736,7 @@
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A218">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B218" t="s">
         <v>1015</v>
@@ -9774,53 +9759,53 @@
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A219">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B219" t="s">
         <v>1020</v>
       </c>
       <c r="C219" t="s">
+        <v>194</v>
+      </c>
+      <c r="D219" t="s">
         <v>1021</v>
       </c>
-      <c r="D219" t="s">
-        <v>1022</v>
-      </c>
       <c r="E219" t="s">
         <v>10</v>
       </c>
       <c r="F219" t="s">
-        <v>1023</v>
+        <v>196</v>
       </c>
       <c r="G219" t="s">
-        <v>1024</v>
+        <v>197</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A220">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B220" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C220" t="s">
+        <v>1023</v>
+      </c>
+      <c r="D220" t="s">
+        <v>1024</v>
+      </c>
+      <c r="E220" t="s">
+        <v>10</v>
+      </c>
+      <c r="F220" t="s">
         <v>1025</v>
       </c>
-      <c r="C220" t="s">
-        <v>194</v>
-      </c>
-      <c r="D220" t="s">
+      <c r="G220" t="s">
         <v>1026</v>
-      </c>
-      <c r="E220" t="s">
-        <v>10</v>
-      </c>
-      <c r="F220" t="s">
-        <v>196</v>
-      </c>
-      <c r="G220" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A221">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B221" t="s">
         <v>1027</v>
@@ -9843,7 +9828,7 @@
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A222">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B222" t="s">
         <v>1032</v>
@@ -9866,7 +9851,7 @@
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A223">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B223" t="s">
         <v>1037</v>
@@ -9889,7 +9874,7 @@
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A224">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B224" t="s">
         <v>1042</v>
@@ -9912,7 +9897,7 @@
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A225">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B225" t="s">
         <v>1047</v>
@@ -9935,76 +9920,76 @@
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A226">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B226" t="s">
         <v>1052</v>
       </c>
       <c r="C226" t="s">
-        <v>1053</v>
+        <v>442</v>
       </c>
       <c r="D226" t="s">
-        <v>1054</v>
+        <v>443</v>
       </c>
       <c r="E226" t="s">
         <v>10</v>
       </c>
       <c r="F226" t="s">
-        <v>1055</v>
+        <v>444</v>
       </c>
       <c r="G226" t="s">
-        <v>1056</v>
+        <v>445</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A227">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B227" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
       <c r="C227" t="s">
-        <v>442</v>
+        <v>14</v>
       </c>
       <c r="D227" t="s">
-        <v>443</v>
+        <v>360</v>
       </c>
       <c r="E227" t="s">
         <v>10</v>
       </c>
       <c r="F227" t="s">
-        <v>444</v>
+        <v>16</v>
       </c>
       <c r="G227" t="s">
-        <v>445</v>
+        <v>17</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A228">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B228" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C228" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D228" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E228" t="s">
+        <v>10</v>
+      </c>
+      <c r="F228" t="s">
+        <v>1057</v>
+      </c>
+      <c r="G228" t="s">
         <v>1058</v>
-      </c>
-      <c r="C228" t="s">
-        <v>14</v>
-      </c>
-      <c r="D228" t="s">
-        <v>360</v>
-      </c>
-      <c r="E228" t="s">
-        <v>10</v>
-      </c>
-      <c r="F228" t="s">
-        <v>16</v>
-      </c>
-      <c r="G228" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A229">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B229" t="s">
         <v>1059</v>
@@ -10027,7 +10012,7 @@
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A230">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B230" t="s">
         <v>1064</v>
@@ -10050,7 +10035,7 @@
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A231">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B231" t="s">
         <v>1069</v>
@@ -10073,7 +10058,7 @@
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A232">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B232" t="s">
         <v>1074</v>
@@ -10096,53 +10081,53 @@
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A233">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B233" t="s">
         <v>1079</v>
       </c>
       <c r="C233" t="s">
+        <v>79</v>
+      </c>
+      <c r="D233" t="s">
         <v>1080</v>
       </c>
-      <c r="D233" t="s">
-        <v>1081</v>
-      </c>
       <c r="E233" t="s">
         <v>10</v>
       </c>
       <c r="F233" t="s">
-        <v>1082</v>
+        <v>81</v>
       </c>
       <c r="G233" t="s">
-        <v>1083</v>
+        <v>82</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A234">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B234" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C234" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D234" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E234" t="s">
+        <v>10</v>
+      </c>
+      <c r="F234" t="s">
         <v>1084</v>
       </c>
-      <c r="C234" t="s">
-        <v>79</v>
-      </c>
-      <c r="D234" t="s">
+      <c r="G234" t="s">
         <v>1085</v>
-      </c>
-      <c r="E234" t="s">
-        <v>10</v>
-      </c>
-      <c r="F234" t="s">
-        <v>81</v>
-      </c>
-      <c r="G234" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A235">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B235" t="s">
         <v>1086</v>
@@ -10165,7 +10150,7 @@
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A236">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B236" t="s">
         <v>1091</v>
@@ -10188,7 +10173,7 @@
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A237">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B237" t="s">
         <v>1096</v>
@@ -10211,7 +10196,7 @@
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A238">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B238" t="s">
         <v>1101</v>
@@ -10234,7 +10219,7 @@
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A239">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B239" t="s">
         <v>1106</v>
@@ -10257,7 +10242,7 @@
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A240">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B240" t="s">
         <v>1111</v>
@@ -10280,7 +10265,7 @@
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A241">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B241" t="s">
         <v>1116</v>
@@ -10303,7 +10288,7 @@
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A242">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B242" t="s">
         <v>1121</v>
@@ -10326,7 +10311,7 @@
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A243">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B243" t="s">
         <v>1126</v>
@@ -10349,7 +10334,7 @@
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A244">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B244" t="s">
         <v>1131</v>
@@ -10372,7 +10357,7 @@
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A245">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B245" t="s">
         <v>1136</v>
@@ -10395,7 +10380,7 @@
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A246">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B246" t="s">
         <v>1141</v>
@@ -10418,7 +10403,7 @@
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A247">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B247" t="s">
         <v>1146</v>
@@ -10441,7 +10426,7 @@
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A248">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B248" t="s">
         <v>1151</v>
@@ -10464,7 +10449,7 @@
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A249">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B249" t="s">
         <v>1156</v>
@@ -10487,7 +10472,7 @@
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A250">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B250" t="s">
         <v>1161</v>
@@ -10510,7 +10495,7 @@
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A251">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B251" t="s">
         <v>1166</v>
@@ -10533,7 +10518,7 @@
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A252">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B252" t="s">
         <v>1171</v>
@@ -10556,7 +10541,7 @@
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A253">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B253" t="s">
         <v>1176</v>
@@ -10579,7 +10564,7 @@
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A254">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B254" t="s">
         <v>1181</v>
@@ -10602,7 +10587,7 @@
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A255">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B255" t="s">
         <v>1186</v>
@@ -10625,7 +10610,7 @@
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A256">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B256" t="s">
         <v>1191</v>
@@ -10648,7 +10633,7 @@
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A257">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B257" t="s">
         <v>1196</v>
@@ -10671,7 +10656,7 @@
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A258">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B258" t="s">
         <v>1201</v>
@@ -10694,7 +10679,7 @@
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A259">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B259" t="s">
         <v>1206</v>
@@ -10717,7 +10702,7 @@
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A260">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B260" t="s">
         <v>1211</v>
@@ -10740,7 +10725,7 @@
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A261">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B261" t="s">
         <v>1216</v>
@@ -10763,7 +10748,7 @@
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A262">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B262" t="s">
         <v>1221</v>
@@ -10786,7 +10771,7 @@
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A263">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B263" t="s">
         <v>1226</v>
@@ -10809,7 +10794,7 @@
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A264">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B264" t="s">
         <v>1231</v>
@@ -10832,7 +10817,7 @@
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A265">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B265" t="s">
         <v>1236</v>
@@ -10855,7 +10840,7 @@
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A266">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B266" t="s">
         <v>1241</v>
@@ -10878,7 +10863,7 @@
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A267">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B267" t="s">
         <v>1246</v>
@@ -10901,7 +10886,7 @@
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A268">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B268" t="s">
         <v>1251</v>
@@ -10924,7 +10909,7 @@
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A269">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B269" t="s">
         <v>1256</v>
@@ -10947,7 +10932,7 @@
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A270">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B270" t="s">
         <v>1261</v>
@@ -10970,7 +10955,7 @@
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A271">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B271" t="s">
         <v>1266</v>
@@ -10993,53 +10978,53 @@
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A272">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B272" t="s">
         <v>1271</v>
       </c>
       <c r="C272" t="s">
-        <v>1272</v>
+        <v>636</v>
       </c>
       <c r="D272" t="s">
-        <v>1273</v>
+        <v>637</v>
       </c>
       <c r="E272" t="s">
         <v>10</v>
       </c>
       <c r="F272" t="s">
-        <v>1274</v>
+        <v>638</v>
       </c>
       <c r="G272" t="s">
-        <v>1275</v>
+        <v>639</v>
       </c>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A273">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B273" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C273" t="s">
+        <v>1273</v>
+      </c>
+      <c r="D273" t="s">
+        <v>1274</v>
+      </c>
+      <c r="E273" t="s">
+        <v>10</v>
+      </c>
+      <c r="F273" t="s">
+        <v>1275</v>
+      </c>
+      <c r="G273" t="s">
         <v>1276</v>
-      </c>
-      <c r="C273" t="s">
-        <v>641</v>
-      </c>
-      <c r="D273" t="s">
-        <v>642</v>
-      </c>
-      <c r="E273" t="s">
-        <v>10</v>
-      </c>
-      <c r="F273" t="s">
-        <v>643</v>
-      </c>
-      <c r="G273" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A274">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B274" t="s">
         <v>1277</v>
@@ -11062,7 +11047,7 @@
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A275">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B275" t="s">
         <v>1282</v>
@@ -11085,7 +11070,7 @@
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A276">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B276" t="s">
         <v>1287</v>
@@ -11104,29 +11089,6 @@
       </c>
       <c r="G276" t="s">
         <v>1291</v>
-      </c>
-    </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A277">
-        <v>275</v>
-      </c>
-      <c r="B277" t="s">
-        <v>1292</v>
-      </c>
-      <c r="C277" t="s">
-        <v>1293</v>
-      </c>
-      <c r="D277" t="s">
-        <v>1294</v>
-      </c>
-      <c r="E277" t="s">
-        <v>10</v>
-      </c>
-      <c r="F277" t="s">
-        <v>1295</v>
-      </c>
-      <c r="G277" t="s">
-        <v>1296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>